<commit_message>
Update file structure for paper
</commit_message>
<xml_diff>
--- a/Archived_simulations.xlsx
+++ b/Archived_simulations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD032EA-D057-4A9A-A430-090E3A1FC5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0398795C-DDA3-4C14-A69F-74CCF5779AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="568">
   <si>
     <t>Date run</t>
   </si>
@@ -1810,6 +1810,87 @@
   </si>
   <si>
     <t>Obj1.2_model.validation_uniform.lambda_target.YOY.R</t>
+  </si>
+  <si>
+    <t>Obj2.1_sample.ALL.ages</t>
+  </si>
+  <si>
+    <t>Does the model work fine to integrate POP relationships?</t>
+  </si>
+  <si>
+    <t>How does the model perform under different sampling schemes (i.e. age classes)?</t>
+  </si>
+  <si>
+    <t>How does the model perform under different sampling intensities?</t>
+  </si>
+  <si>
+    <t>Test different sampling schemes for CKMR</t>
+  </si>
+  <si>
+    <t>Obj2.1_sample.ALL.ages.R</t>
+  </si>
+  <si>
+    <t>Obj2.1_target.YOY</t>
+  </si>
+  <si>
+    <t>Obj2.1_target.YOY.R</t>
+  </si>
+  <si>
+    <t>Obj2.1_sample.all.juveniles</t>
+  </si>
+  <si>
+    <t>Obj2.1_sample.all.juveniles.R</t>
+  </si>
+  <si>
+    <t>lambda.1</t>
+  </si>
+  <si>
+    <t>Obj1.2_PopSimLambda.1_uniform.lambda.prior</t>
+  </si>
+  <si>
+    <t>How do the diffuse prior results compare to the informed prior results?</t>
+  </si>
+  <si>
+    <t>Obj1.2_PopSimLambda.1_uniform.lambda.prior.R</t>
+  </si>
+  <si>
+    <t>lambda.variable</t>
+  </si>
+  <si>
+    <t>Obj1.2_PopSimLambda.variable_uniform.lambda.prior</t>
+  </si>
+  <si>
+    <t>Obj1.2_PopSimLambda.variable_uniform.lambda.prior.R</t>
+  </si>
+  <si>
+    <t>Obj1.2_PopSimLambda.1_fixed.lambda.prior</t>
+  </si>
+  <si>
+    <t>Obj1.2_PopSimLambda.1_fixed.lambda.prior.R</t>
+  </si>
+  <si>
+    <t>Obj1.2_PopSimLambda.variable_fixed.lambda.prior</t>
+  </si>
+  <si>
+    <t>Obj1.2_PopSimLambda.variable_fixed.lambda.prior.R</t>
+  </si>
+  <si>
+    <t>uniform: 0.5 - 0.99</t>
+  </si>
+  <si>
+    <t>truth</t>
+  </si>
+  <si>
+    <t>Obj1.1_model.validation</t>
+  </si>
+  <si>
+    <t>Does the model perform as expected when we set an informed prior on lambda and survival?</t>
+  </si>
+  <si>
+    <t>Validate model using informed priors</t>
+  </si>
+  <si>
+    <t>Obj1.1_model.validation.R</t>
   </si>
 </sst>
 </file>
@@ -3223,33 +3304,33 @@
       <selection pane="topRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="39.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="31.5703125" customWidth="1"/>
     <col min="16" max="16" width="51" customWidth="1"/>
-    <col min="17" max="17" width="49.6640625" style="35" customWidth="1"/>
-    <col min="18" max="21" width="19.5546875" customWidth="1"/>
-    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="17" max="17" width="49.7109375" style="35" customWidth="1"/>
+    <col min="18" max="21" width="19.5703125" customWidth="1"/>
+    <col min="22" max="23" width="25.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="89" t="s">
         <v>105</v>
       </c>
@@ -3338,7 +3419,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="90" t="s">
         <v>106</v>
       </c>
@@ -3389,7 +3470,7 @@
       <c r="AB2" s="59"/>
       <c r="AC2" s="60"/>
     </row>
-    <row r="3" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>107</v>
       </c>
@@ -3440,7 +3521,7 @@
       <c r="AB3" s="61"/>
       <c r="AC3" s="62"/>
     </row>
-    <row r="4" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>108</v>
       </c>
@@ -3491,7 +3572,7 @@
       <c r="AB4" s="61"/>
       <c r="AC4" s="62"/>
     </row>
-    <row r="5" spans="1:29" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>115</v>
       </c>
@@ -3540,7 +3621,7 @@
       <c r="AB5" s="61"/>
       <c r="AC5" s="62"/>
     </row>
-    <row r="6" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>116</v>
       </c>
@@ -3593,7 +3674,7 @@
       <c r="AB6" s="61"/>
       <c r="AC6" s="62"/>
     </row>
-    <row r="7" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>117</v>
       </c>
@@ -3640,7 +3721,7 @@
       <c r="AB7" s="61"/>
       <c r="AC7" s="62"/>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>128</v>
       </c>
@@ -3673,7 +3754,7 @@
       <c r="AB8" s="61"/>
       <c r="AC8" s="62"/>
     </row>
-    <row r="9" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>129</v>
       </c>
@@ -3720,7 +3801,7 @@
       <c r="AB9" s="63"/>
       <c r="AC9" s="64"/>
     </row>
-    <row r="10" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>131</v>
       </c>
@@ -3777,7 +3858,7 @@
       <c r="AB10" s="63"/>
       <c r="AC10" s="64"/>
     </row>
-    <row r="11" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>144</v>
       </c>
@@ -3830,7 +3911,7 @@
       <c r="AB11" s="63"/>
       <c r="AC11" s="64"/>
     </row>
-    <row r="12" spans="1:29" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>146</v>
       </c>
@@ -3889,7 +3970,7 @@
       <c r="AB12" s="63"/>
       <c r="AC12" s="64"/>
     </row>
-    <row r="13" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>152</v>
       </c>
@@ -3950,7 +4031,7 @@
       <c r="AB13" s="63"/>
       <c r="AC13" s="64"/>
     </row>
-    <row r="14" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>178</v>
       </c>
@@ -4009,7 +4090,7 @@
       <c r="AB14" s="65"/>
       <c r="AC14" s="66"/>
     </row>
-    <row r="15" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>134</v>
       </c>
@@ -4070,7 +4151,7 @@
       <c r="AB15" s="63"/>
       <c r="AC15" s="64"/>
     </row>
-    <row r="16" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>134</v>
       </c>
@@ -4131,7 +4212,7 @@
       <c r="AB16" s="65"/>
       <c r="AC16" s="66"/>
     </row>
-    <row r="17" spans="1:29" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>193</v>
       </c>
@@ -4194,7 +4275,7 @@
       <c r="AB17" s="65"/>
       <c r="AC17" s="66"/>
     </row>
-    <row r="18" spans="1:29" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>202</v>
       </c>
@@ -4243,7 +4324,7 @@
       <c r="AB18" s="65"/>
       <c r="AC18" s="66"/>
     </row>
-    <row r="19" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>202</v>
       </c>
@@ -4292,7 +4373,7 @@
       <c r="AB19" s="65"/>
       <c r="AC19" s="66"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>205</v>
       </c>
@@ -4327,7 +4408,7 @@
       <c r="AB20" s="65"/>
       <c r="AC20" s="66"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="11"/>
@@ -4358,7 +4439,7 @@
       <c r="AB21" s="65"/>
       <c r="AC21" s="66"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="11"/>
@@ -4389,7 +4470,7 @@
       <c r="AB22" s="65"/>
       <c r="AC22" s="66"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="11"/>
@@ -4420,7 +4501,7 @@
       <c r="AB23" s="65"/>
       <c r="AC23" s="66"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="11"/>
@@ -4451,7 +4532,7 @@
       <c r="AB24" s="65"/>
       <c r="AC24" s="66"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="11"/>
@@ -4482,7 +4563,7 @@
       <c r="AB25" s="65"/>
       <c r="AC25" s="66"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="11"/>
@@ -4513,7 +4594,7 @@
       <c r="AB26" s="65"/>
       <c r="AC26" s="66"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="11"/>
@@ -4544,7 +4625,7 @@
       <c r="AB27" s="65"/>
       <c r="AC27" s="66"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="11"/>
@@ -4575,7 +4656,7 @@
       <c r="AB28" s="65"/>
       <c r="AC28" s="66"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="11"/>
@@ -4606,7 +4687,7 @@
       <c r="AB29" s="65"/>
       <c r="AC29" s="66"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="11"/>
@@ -4637,7 +4718,7 @@
       <c r="AB30" s="65"/>
       <c r="AC30" s="66"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="11"/>
@@ -4668,7 +4749,7 @@
       <c r="AB31" s="65"/>
       <c r="AC31" s="66"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="11"/>
@@ -4699,7 +4780,7 @@
       <c r="AB32" s="65"/>
       <c r="AC32" s="66"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="11"/>
@@ -4730,7 +4811,7 @@
       <c r="AB33" s="65"/>
       <c r="AC33" s="66"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="11"/>
@@ -4761,7 +4842,7 @@
       <c r="AB34" s="65"/>
       <c r="AC34" s="66"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="11"/>
@@ -4792,7 +4873,7 @@
       <c r="AB35" s="65"/>
       <c r="AC35" s="66"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="11"/>
@@ -4823,7 +4904,7 @@
       <c r="AB36" s="65"/>
       <c r="AC36" s="66"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="11"/>
@@ -4854,7 +4935,7 @@
       <c r="AB37" s="65"/>
       <c r="AC37" s="66"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="11"/>
@@ -4885,7 +4966,7 @@
       <c r="AB38" s="65"/>
       <c r="AC38" s="66"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="11"/>
@@ -4916,7 +4997,7 @@
       <c r="AB39" s="65"/>
       <c r="AC39" s="66"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="11"/>
@@ -4947,7 +5028,7 @@
       <c r="AB40" s="65"/>
       <c r="AC40" s="66"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="11"/>
@@ -4978,7 +5059,7 @@
       <c r="AB41" s="65"/>
       <c r="AC41" s="66"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="11"/>
@@ -5009,7 +5090,7 @@
       <c r="AB42" s="65"/>
       <c r="AC42" s="66"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="11"/>
@@ -5040,7 +5121,7 @@
       <c r="AB43" s="65"/>
       <c r="AC43" s="66"/>
     </row>
-    <row r="44" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="92"/>
@@ -5099,14 +5180,14 @@
       <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="105.88671875" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="1" max="1" width="105.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -5117,7 +5198,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>93</v>
       </c>
@@ -5128,7 +5209,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>62</v>
       </c>
@@ -5136,7 +5217,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>64</v>
       </c>
@@ -5144,7 +5225,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>86</v>
       </c>
@@ -5152,19 +5233,19 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="35"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="35"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="35"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="35"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="35"/>
     </row>
   </sheetData>
@@ -5181,24 +5262,24 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="36.109375" customWidth="1"/>
-    <col min="7" max="7" width="38.5546875" customWidth="1"/>
-    <col min="8" max="8" width="48.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="11" width="14.88671875" customWidth="1"/>
-    <col min="12" max="12" width="24.6640625" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" customWidth="1"/>
+    <col min="7" max="7" width="38.5703125" customWidth="1"/>
+    <col min="8" max="8" width="48.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="11" width="14.85546875" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>319</v>
       </c>
@@ -5232,7 +5313,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>322</v>
       </c>
@@ -5261,7 +5342,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>323</v>
       </c>
@@ -5290,7 +5371,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>324</v>
       </c>
@@ -5319,7 +5400,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>325</v>
       </c>
@@ -5330,7 +5411,7 @@
       <c r="G5" s="135"/>
       <c r="H5" s="136"/>
     </row>
-    <row r="6" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>323</v>
       </c>
@@ -5359,7 +5440,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7" s="35"/>
       <c r="D7" s="35"/>
       <c r="E7" s="35"/>
@@ -5367,7 +5448,7 @@
       <c r="G7" s="135"/>
       <c r="H7" s="136"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
       <c r="E8" s="35"/>
@@ -5375,7 +5456,7 @@
       <c r="G8" s="135"/>
       <c r="H8" s="136"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
@@ -5383,7 +5464,7 @@
       <c r="G9" s="135"/>
       <c r="H9" s="136"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
@@ -5391,7 +5472,7 @@
       <c r="G10" s="135"/>
       <c r="H10" s="136"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
@@ -5399,7 +5480,7 @@
       <c r="G11" s="135"/>
       <c r="H11" s="136"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
       <c r="E12" s="35"/>
@@ -5407,7 +5488,7 @@
       <c r="G12" s="135"/>
       <c r="H12" s="136"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
       <c r="E13" s="35"/>
@@ -5415,391 +5496,391 @@
       <c r="G13" s="135"/>
       <c r="H13" s="136"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G14" s="135"/>
       <c r="H14" s="136"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G15" s="135"/>
       <c r="H15" s="136"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G16" s="135"/>
       <c r="H16" s="136"/>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G17" s="135"/>
       <c r="H17" s="135"/>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G18" s="135"/>
       <c r="H18" s="135"/>
     </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G19" s="135"/>
       <c r="H19" s="135"/>
     </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G20" s="135"/>
       <c r="H20" s="135"/>
     </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G21" s="135"/>
       <c r="H21" s="135"/>
     </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G22" s="135"/>
       <c r="H22" s="135"/>
     </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G23" s="135"/>
       <c r="H23" s="135"/>
     </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G24" s="135"/>
       <c r="H24" s="135"/>
     </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G25" s="135"/>
       <c r="H25" s="135"/>
     </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G26" s="135"/>
       <c r="H26" s="135"/>
     </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G27" s="135"/>
       <c r="H27" s="135"/>
     </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G28" s="135"/>
       <c r="H28" s="135"/>
     </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G29" s="135"/>
       <c r="H29" s="135"/>
     </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G30" s="135"/>
       <c r="H30" s="135"/>
     </row>
-    <row r="31" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G31" s="135"/>
       <c r="H31" s="135"/>
     </row>
-    <row r="32" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G32" s="135"/>
       <c r="H32" s="135"/>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G33" s="135"/>
       <c r="H33" s="135"/>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G34" s="135"/>
       <c r="H34" s="135"/>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G35" s="135"/>
       <c r="H35" s="135"/>
     </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G36" s="135"/>
       <c r="H36" s="135"/>
     </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G37" s="135"/>
       <c r="H37" s="135"/>
     </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G38" s="135"/>
       <c r="H38" s="135"/>
     </row>
-    <row r="39" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G39" s="135"/>
       <c r="H39" s="135"/>
     </row>
-    <row r="40" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G40" s="135"/>
       <c r="H40" s="135"/>
     </row>
-    <row r="41" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G41" s="135"/>
       <c r="H41" s="135"/>
     </row>
-    <row r="42" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G42" s="135"/>
       <c r="H42" s="135"/>
     </row>
-    <row r="43" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G43" s="135"/>
       <c r="H43" s="135"/>
     </row>
-    <row r="44" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G44" s="135"/>
       <c r="H44" s="135"/>
     </row>
-    <row r="45" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G45" s="135"/>
       <c r="H45" s="135"/>
     </row>
-    <row r="46" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G46" s="135"/>
       <c r="H46" s="135"/>
     </row>
-    <row r="47" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G47" s="135"/>
       <c r="H47" s="135"/>
     </row>
-    <row r="48" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G48" s="135"/>
       <c r="H48" s="135"/>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G49" s="135"/>
       <c r="H49" s="135"/>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G50" s="135"/>
       <c r="H50" s="135"/>
     </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G51" s="135"/>
       <c r="H51" s="135"/>
     </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G52" s="135"/>
       <c r="H52" s="135"/>
     </row>
-    <row r="53" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G53" s="135"/>
       <c r="H53" s="135"/>
     </row>
-    <row r="54" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G54" s="135"/>
       <c r="H54" s="135"/>
     </row>
-    <row r="55" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G55" s="135"/>
       <c r="H55" s="135"/>
     </row>
-    <row r="56" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G56" s="135"/>
       <c r="H56" s="135"/>
     </row>
-    <row r="57" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G57" s="135"/>
       <c r="H57" s="135"/>
     </row>
-    <row r="58" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G58" s="135"/>
       <c r="H58" s="135"/>
     </row>
-    <row r="59" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G59" s="135"/>
       <c r="H59" s="135"/>
     </row>
-    <row r="60" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G60" s="135"/>
       <c r="H60" s="135"/>
     </row>
-    <row r="61" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G61" s="135"/>
       <c r="H61" s="135"/>
     </row>
-    <row r="62" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G62" s="135"/>
       <c r="H62" s="135"/>
     </row>
-    <row r="63" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G63" s="135"/>
       <c r="H63" s="135"/>
     </row>
-    <row r="64" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G64" s="135"/>
       <c r="H64" s="135"/>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G65" s="135"/>
       <c r="H65" s="135"/>
     </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G66" s="135"/>
       <c r="H66" s="135"/>
     </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G67" s="135"/>
       <c r="H67" s="135"/>
     </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G68" s="135"/>
       <c r="H68" s="135"/>
     </row>
-    <row r="69" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G69" s="135"/>
       <c r="H69" s="135"/>
     </row>
-    <row r="70" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G70" s="135"/>
       <c r="H70" s="135"/>
     </row>
-    <row r="71" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G71" s="135"/>
       <c r="H71" s="135"/>
     </row>
-    <row r="72" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G72" s="135"/>
       <c r="H72" s="135"/>
     </row>
-    <row r="73" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G73" s="135"/>
       <c r="H73" s="135"/>
     </row>
-    <row r="74" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G74" s="135"/>
       <c r="H74" s="135"/>
     </row>
-    <row r="75" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G75" s="135"/>
       <c r="H75" s="135"/>
     </row>
-    <row r="76" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G76" s="135"/>
       <c r="H76" s="135"/>
     </row>
-    <row r="77" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G77" s="135"/>
       <c r="H77" s="135"/>
     </row>
-    <row r="78" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G78" s="135"/>
       <c r="H78" s="135"/>
     </row>
-    <row r="79" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G79" s="135"/>
       <c r="H79" s="135"/>
     </row>
-    <row r="80" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G80" s="135"/>
       <c r="H80" s="135"/>
     </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G81" s="135"/>
       <c r="H81" s="135"/>
     </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G82" s="135"/>
       <c r="H82" s="135"/>
     </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G83" s="135"/>
       <c r="H83" s="135"/>
     </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G84" s="135"/>
       <c r="H84" s="135"/>
     </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G85" s="135"/>
       <c r="H85" s="135"/>
     </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G86" s="135"/>
       <c r="H86" s="135"/>
     </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G87" s="135"/>
       <c r="H87" s="135"/>
     </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G88" s="135"/>
       <c r="H88" s="135"/>
     </row>
-    <row r="89" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G89" s="135"/>
       <c r="H89" s="135"/>
     </row>
-    <row r="90" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G90" s="135"/>
       <c r="H90" s="135"/>
     </row>
-    <row r="91" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G91" s="135"/>
       <c r="H91" s="135"/>
     </row>
-    <row r="92" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G92" s="135"/>
       <c r="H92" s="135"/>
     </row>
-    <row r="93" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G93" s="135"/>
       <c r="H93" s="135"/>
     </row>
-    <row r="94" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G94" s="135"/>
       <c r="H94" s="135"/>
     </row>
-    <row r="95" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G95" s="135"/>
       <c r="H95" s="135"/>
     </row>
-    <row r="96" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G96" s="135"/>
       <c r="H96" s="135"/>
     </row>
-    <row r="97" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G97" s="135"/>
       <c r="H97" s="135"/>
     </row>
-    <row r="98" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G98" s="135"/>
       <c r="H98" s="135"/>
     </row>
-    <row r="99" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G99" s="135"/>
       <c r="H99" s="135"/>
     </row>
-    <row r="100" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G100" s="135"/>
       <c r="H100" s="135"/>
     </row>
-    <row r="101" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G101" s="135"/>
       <c r="H101" s="135"/>
     </row>
-    <row r="102" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G102" s="135"/>
       <c r="H102" s="135"/>
     </row>
-    <row r="103" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G103" s="135"/>
       <c r="H103" s="135"/>
     </row>
-    <row r="104" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G104" s="135"/>
       <c r="H104" s="135"/>
     </row>
-    <row r="105" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G105" s="135"/>
       <c r="H105" s="135"/>
     </row>
-    <row r="106" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G106" s="135"/>
       <c r="H106" s="135"/>
     </row>
-    <row r="107" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G107" s="135"/>
       <c r="H107" s="135"/>
     </row>
-    <row r="108" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G108" s="135"/>
       <c r="H108" s="135"/>
     </row>
-    <row r="109" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G109" s="135"/>
       <c r="H109" s="135"/>
     </row>
-    <row r="110" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G110" s="135"/>
       <c r="H110" s="135"/>
     </row>
@@ -5817,15 +5898,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="5" width="73.88671875" customWidth="1"/>
-    <col min="6" max="6" width="41.88671875" customWidth="1"/>
+    <col min="2" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="5" width="73.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="134" t="s">
         <v>306</v>
       </c>
@@ -5845,7 +5926,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="132">
         <v>1</v>
       </c>
@@ -5861,7 +5942,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="132">
         <v>2.1</v>
       </c>
@@ -5877,7 +5958,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="132">
         <v>2.2000000000000002</v>
       </c>
@@ -5893,7 +5974,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="132">
         <v>3</v>
       </c>
@@ -5906,7 +5987,7 @@
       </c>
       <c r="E5" s="135"/>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="132">
         <v>4</v>
       </c>
@@ -5919,217 +6000,217 @@
       </c>
       <c r="E6" s="135"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="132"/>
       <c r="B7" s="132"/>
       <c r="C7" s="132"/>
       <c r="D7" s="135"/>
       <c r="E7" s="135"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="132"/>
       <c r="B8" s="132"/>
       <c r="C8" s="132"/>
       <c r="D8" s="135"/>
       <c r="E8" s="135"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="132"/>
       <c r="B9" s="132"/>
       <c r="C9" s="132"/>
       <c r="D9" s="135"/>
       <c r="E9" s="135"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="132"/>
       <c r="B10" s="132"/>
       <c r="C10" s="132"/>
       <c r="D10" s="135"/>
       <c r="E10" s="135"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="132"/>
       <c r="B11" s="132"/>
       <c r="C11" s="132"/>
       <c r="D11" s="135"/>
       <c r="E11" s="135"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="132"/>
       <c r="B12" s="132"/>
       <c r="C12" s="132"/>
       <c r="D12" s="135"/>
       <c r="E12" s="135"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="132"/>
       <c r="B13" s="132"/>
       <c r="C13" s="132"/>
       <c r="D13" s="135"/>
       <c r="E13" s="135"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="132"/>
       <c r="B14" s="132"/>
       <c r="C14" s="132"/>
       <c r="D14" s="135"/>
       <c r="E14" s="135"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="132"/>
       <c r="B15" s="132"/>
       <c r="C15" s="132"/>
       <c r="D15" s="135"/>
       <c r="E15" s="135"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="132"/>
       <c r="B16" s="132"/>
       <c r="C16" s="132"/>
       <c r="D16" s="135"/>
       <c r="E16" s="135"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="132"/>
       <c r="B17" s="132"/>
       <c r="C17" s="132"/>
       <c r="D17" s="135"/>
       <c r="E17" s="135"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="132"/>
       <c r="B18" s="132"/>
       <c r="C18" s="132"/>
       <c r="D18" s="135"/>
       <c r="E18" s="135"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="132"/>
       <c r="B19" s="132"/>
       <c r="C19" s="132"/>
       <c r="D19" s="135"/>
       <c r="E19" s="135"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="132"/>
       <c r="B20" s="132"/>
       <c r="C20" s="132"/>
       <c r="D20" s="135"/>
       <c r="E20" s="135"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="132"/>
       <c r="B21" s="132"/>
       <c r="C21" s="132"/>
       <c r="D21" s="135"/>
       <c r="E21" s="135"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="132"/>
       <c r="B22" s="132"/>
       <c r="C22" s="132"/>
       <c r="D22" s="135"/>
       <c r="E22" s="135"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="132"/>
       <c r="B23" s="132"/>
       <c r="C23" s="132"/>
       <c r="D23" s="135"/>
       <c r="E23" s="135"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="132"/>
       <c r="B24" s="132"/>
       <c r="C24" s="132"/>
       <c r="D24" s="135"/>
       <c r="E24" s="135"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25" s="35"/>
       <c r="E25" s="35"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" s="35"/>
       <c r="E26" s="35"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" s="35"/>
       <c r="E27" s="35"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" s="35"/>
       <c r="E28" s="35"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" s="35"/>
       <c r="E29" s="35"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30" s="35"/>
       <c r="E30" s="35"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D31" s="35"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32" s="35"/>
       <c r="E32" s="35"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" s="35"/>
       <c r="E33" s="35"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" s="35"/>
       <c r="E34" s="35"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" s="35"/>
       <c r="E35" s="35"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" s="35"/>
       <c r="E36" s="35"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" s="35"/>
       <c r="E38" s="35"/>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39" s="35"/>
       <c r="E39" s="35"/>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D42" s="35"/>
       <c r="E42" s="35"/>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D43" s="35"/>
       <c r="E43" s="35"/>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44" s="35"/>
       <c r="E44" s="35"/>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D45" s="35"/>
       <c r="E45" s="35"/>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D46" s="35"/>
       <c r="E46" s="35"/>
     </row>
@@ -6147,13 +6228,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>161</v>
       </c>
@@ -6161,7 +6242,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>280</v>
       </c>
@@ -6169,7 +6250,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>308</v>
       </c>
@@ -6177,7 +6258,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
@@ -6185,7 +6266,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>327</v>
       </c>
@@ -6193,10 +6274,10 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="35"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="35"/>
     </row>
   </sheetData>
@@ -6213,32 +6294,32 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="39.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="51" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="31.5546875" customWidth="1"/>
-    <col min="17" max="20" width="19.5546875" customWidth="1"/>
-    <col min="21" max="22" width="25.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="31.5703125" customWidth="1"/>
+    <col min="17" max="20" width="19.5703125" customWidth="1"/>
+    <col min="21" max="22" width="25.28515625" customWidth="1"/>
     <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="89" t="s">
         <v>105</v>
       </c>
@@ -6324,7 +6405,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>268</v>
       </c>
@@ -6372,7 +6453,7 @@
       <c r="AA2" s="63"/>
       <c r="AB2" s="64"/>
     </row>
-    <row r="3" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>274</v>
       </c>
@@ -6422,7 +6503,7 @@
       <c r="AA3" s="65"/>
       <c r="AB3" s="66"/>
     </row>
-    <row r="4" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>298</v>
       </c>
@@ -6470,7 +6551,7 @@
       <c r="AA4" s="65"/>
       <c r="AB4" s="66"/>
     </row>
-    <row r="5" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>299</v>
       </c>
@@ -6518,7 +6599,7 @@
       <c r="AA5" s="65"/>
       <c r="AB5" s="66"/>
     </row>
-    <row r="6" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>294</v>
       </c>
@@ -6566,7 +6647,7 @@
       <c r="AA6" s="65"/>
       <c r="AB6" s="66"/>
     </row>
-    <row r="7" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>296</v>
       </c>
@@ -6614,7 +6695,7 @@
       <c r="AA7" s="65"/>
       <c r="AB7" s="66"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="11"/>
@@ -6644,7 +6725,7 @@
       <c r="AA8" s="65"/>
       <c r="AB8" s="66"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="11"/>
@@ -6674,7 +6755,7 @@
       <c r="AA9" s="65"/>
       <c r="AB9" s="66"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="11"/>
@@ -6704,7 +6785,7 @@
       <c r="AA10" s="65"/>
       <c r="AB10" s="66"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="11"/>
@@ -6734,7 +6815,7 @@
       <c r="AA11" s="65"/>
       <c r="AB11" s="66"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="11"/>
@@ -6764,7 +6845,7 @@
       <c r="AA12" s="65"/>
       <c r="AB12" s="66"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="11"/>
@@ -6794,7 +6875,7 @@
       <c r="AA13" s="65"/>
       <c r="AB13" s="66"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="11"/>
@@ -6824,7 +6905,7 @@
       <c r="AA14" s="65"/>
       <c r="AB14" s="66"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="11"/>
@@ -6854,7 +6935,7 @@
       <c r="AA15" s="65"/>
       <c r="AB15" s="66"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="11"/>
@@ -6884,7 +6965,7 @@
       <c r="AA16" s="65"/>
       <c r="AB16" s="66"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="11"/>
@@ -6914,7 +6995,7 @@
       <c r="AA17" s="65"/>
       <c r="AB17" s="66"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="11"/>
@@ -6944,7 +7025,7 @@
       <c r="AA18" s="65"/>
       <c r="AB18" s="66"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="11"/>
@@ -6974,7 +7055,7 @@
       <c r="AA19" s="65"/>
       <c r="AB19" s="66"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="11"/>
@@ -7004,7 +7085,7 @@
       <c r="AA20" s="65"/>
       <c r="AB20" s="66"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="11"/>
@@ -7034,7 +7115,7 @@
       <c r="AA21" s="65"/>
       <c r="AB21" s="66"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="11"/>
@@ -7064,7 +7145,7 @@
       <c r="AA22" s="65"/>
       <c r="AB22" s="66"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="11"/>
@@ -7094,7 +7175,7 @@
       <c r="AA23" s="65"/>
       <c r="AB23" s="66"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="11"/>
@@ -7124,7 +7205,7 @@
       <c r="AA24" s="65"/>
       <c r="AB24" s="66"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="11"/>
@@ -7154,7 +7235,7 @@
       <c r="AA25" s="65"/>
       <c r="AB25" s="66"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="11"/>
@@ -7184,7 +7265,7 @@
       <c r="AA26" s="65"/>
       <c r="AB26" s="66"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="11"/>
@@ -7214,7 +7295,7 @@
       <c r="AA27" s="65"/>
       <c r="AB27" s="66"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="11"/>
@@ -7244,7 +7325,7 @@
       <c r="AA28" s="65"/>
       <c r="AB28" s="66"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="11"/>
@@ -7274,7 +7355,7 @@
       <c r="AA29" s="65"/>
       <c r="AB29" s="66"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="11"/>
@@ -7304,7 +7385,7 @@
       <c r="AA30" s="65"/>
       <c r="AB30" s="66"/>
     </row>
-    <row r="31" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="92"/>
@@ -7334,77 +7415,77 @@
       <c r="AA31" s="67"/>
       <c r="AB31" s="68"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="K32" s="35"/>
       <c r="M32" s="35"/>
       <c r="N32" s="35"/>
       <c r="O32" s="35"/>
       <c r="P32" s="35"/>
     </row>
-    <row r="33" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K33" s="35"/>
       <c r="M33" s="35"/>
       <c r="N33" s="35"/>
       <c r="O33" s="35"/>
       <c r="P33" s="35"/>
     </row>
-    <row r="34" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K34" s="35"/>
       <c r="M34" s="35"/>
       <c r="N34" s="35"/>
       <c r="O34" s="35"/>
       <c r="P34" s="35"/>
     </row>
-    <row r="35" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K35" s="35"/>
       <c r="M35" s="35"/>
       <c r="N35" s="35"/>
       <c r="O35" s="35"/>
       <c r="P35" s="35"/>
     </row>
-    <row r="36" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K36" s="35"/>
       <c r="M36" s="35"/>
       <c r="N36" s="35"/>
       <c r="O36" s="35"/>
       <c r="P36" s="35"/>
     </row>
-    <row r="37" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K37" s="35"/>
       <c r="M37" s="35"/>
       <c r="N37" s="35"/>
       <c r="O37" s="35"/>
       <c r="P37" s="35"/>
     </row>
-    <row r="38" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K38" s="35"/>
       <c r="M38" s="35"/>
       <c r="N38" s="35"/>
       <c r="O38" s="35"/>
       <c r="P38" s="35"/>
     </row>
-    <row r="39" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K39" s="35"/>
       <c r="M39" s="35"/>
       <c r="N39" s="35"/>
       <c r="O39" s="35"/>
       <c r="P39" s="35"/>
     </row>
-    <row r="40" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K40" s="35"/>
       <c r="M40" s="35"/>
       <c r="N40" s="35"/>
       <c r="O40" s="35"/>
       <c r="P40" s="35"/>
     </row>
-    <row r="41" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K41" s="35"/>
       <c r="M41" s="35"/>
       <c r="N41" s="35"/>
       <c r="O41" s="35"/>
       <c r="P41" s="35"/>
     </row>
-    <row r="42" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K42" s="35"/>
       <c r="M42" s="35"/>
       <c r="N42" s="35"/>
@@ -7430,32 +7511,32 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="20.109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="39.5546875" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="51" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="31.5546875" customWidth="1"/>
-    <col min="18" max="21" width="19.5546875" customWidth="1"/>
-    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="31.5703125" customWidth="1"/>
+    <col min="18" max="21" width="19.5703125" customWidth="1"/>
+    <col min="22" max="23" width="25.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="89" t="s">
         <v>105</v>
       </c>
@@ -7544,7 +7625,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="90" t="s">
         <v>213</v>
       </c>
@@ -7605,7 +7686,7 @@
       <c r="AB2" s="59"/>
       <c r="AC2" s="60"/>
     </row>
-    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>221</v>
       </c>
@@ -7666,7 +7747,7 @@
       <c r="AB3" s="61"/>
       <c r="AC3" s="62"/>
     </row>
-    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>220</v>
       </c>
@@ -7727,7 +7808,7 @@
       <c r="AB4" s="61"/>
       <c r="AC4" s="62"/>
     </row>
-    <row r="5" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>219</v>
       </c>
@@ -7788,7 +7869,7 @@
       <c r="AB5" s="61"/>
       <c r="AC5" s="62"/>
     </row>
-    <row r="6" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>213</v>
       </c>
@@ -7851,7 +7932,7 @@
       <c r="AB6" s="61"/>
       <c r="AC6" s="62"/>
     </row>
-    <row r="7" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>242</v>
       </c>
@@ -7914,7 +7995,7 @@
       <c r="AB7" s="61"/>
       <c r="AC7" s="62"/>
     </row>
-    <row r="8" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>221</v>
       </c>
@@ -7977,7 +8058,7 @@
       <c r="AB8" s="61"/>
       <c r="AC8" s="62"/>
     </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>213</v>
       </c>
@@ -8030,7 +8111,7 @@
       <c r="AB9" s="61"/>
       <c r="AC9" s="62"/>
     </row>
-    <row r="10" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>242</v>
       </c>
@@ -8083,7 +8164,7 @@
       <c r="AB10" s="61"/>
       <c r="AC10" s="62"/>
     </row>
-    <row r="11" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>221</v>
       </c>
@@ -8136,7 +8217,7 @@
       <c r="AB11" s="61"/>
       <c r="AC11" s="62"/>
     </row>
-    <row r="12" spans="1:29" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>260</v>
       </c>
@@ -8191,7 +8272,7 @@
       <c r="AB12" s="63"/>
       <c r="AC12" s="64"/>
     </row>
-    <row r="13" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>269</v>
       </c>
@@ -8244,7 +8325,7 @@
       <c r="AB13" s="63"/>
       <c r="AC13" s="64"/>
     </row>
-    <row r="14" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>270</v>
       </c>
@@ -8297,7 +8378,7 @@
       <c r="AB14" s="65"/>
       <c r="AC14" s="66"/>
     </row>
-    <row r="15" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>271</v>
       </c>
@@ -8350,7 +8431,7 @@
       <c r="AB15" s="63"/>
       <c r="AC15" s="64"/>
     </row>
-    <row r="16" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>275</v>
       </c>
@@ -8401,7 +8482,7 @@
       <c r="AB16" s="65"/>
       <c r="AC16" s="66"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="11"/>
@@ -8432,7 +8513,7 @@
       <c r="AB17" s="65"/>
       <c r="AC17" s="66"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="11"/>
@@ -8463,7 +8544,7 @@
       <c r="AB18" s="65"/>
       <c r="AC18" s="66"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="11"/>
@@ -8494,7 +8575,7 @@
       <c r="AB19" s="65"/>
       <c r="AC19" s="66"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="11"/>
@@ -8525,7 +8606,7 @@
       <c r="AB20" s="65"/>
       <c r="AC20" s="66"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="11"/>
@@ -8556,7 +8637,7 @@
       <c r="AB21" s="65"/>
       <c r="AC21" s="66"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="11"/>
@@ -8587,7 +8668,7 @@
       <c r="AB22" s="65"/>
       <c r="AC22" s="66"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="11"/>
@@ -8618,7 +8699,7 @@
       <c r="AB23" s="65"/>
       <c r="AC23" s="66"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="11"/>
@@ -8649,7 +8730,7 @@
       <c r="AB24" s="65"/>
       <c r="AC24" s="66"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="11"/>
@@ -8680,7 +8761,7 @@
       <c r="AB25" s="65"/>
       <c r="AC25" s="66"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="11"/>
@@ -8711,7 +8792,7 @@
       <c r="AB26" s="65"/>
       <c r="AC26" s="66"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="11"/>
@@ -8742,7 +8823,7 @@
       <c r="AB27" s="65"/>
       <c r="AC27" s="66"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="11"/>
@@ -8773,7 +8854,7 @@
       <c r="AB28" s="65"/>
       <c r="AC28" s="66"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="11"/>
@@ -8804,7 +8885,7 @@
       <c r="AB29" s="65"/>
       <c r="AC29" s="66"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="11"/>
@@ -8835,7 +8916,7 @@
       <c r="AB30" s="65"/>
       <c r="AC30" s="66"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="11"/>
@@ -8866,7 +8947,7 @@
       <c r="AB31" s="65"/>
       <c r="AC31" s="66"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="11"/>
@@ -8897,7 +8978,7 @@
       <c r="AB32" s="65"/>
       <c r="AC32" s="66"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="11"/>
@@ -8928,7 +9009,7 @@
       <c r="AB33" s="65"/>
       <c r="AC33" s="66"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="11"/>
@@ -8959,7 +9040,7 @@
       <c r="AB34" s="65"/>
       <c r="AC34" s="66"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="11"/>
@@ -8990,7 +9071,7 @@
       <c r="AB35" s="65"/>
       <c r="AC35" s="66"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="11"/>
@@ -9021,7 +9102,7 @@
       <c r="AB36" s="65"/>
       <c r="AC36" s="66"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="11"/>
@@ -9052,7 +9133,7 @@
       <c r="AB37" s="65"/>
       <c r="AC37" s="66"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="11"/>
@@ -9083,7 +9164,7 @@
       <c r="AB38" s="65"/>
       <c r="AC38" s="66"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="11"/>
@@ -9114,7 +9195,7 @@
       <c r="AB39" s="65"/>
       <c r="AC39" s="66"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="11"/>
@@ -9145,7 +9226,7 @@
       <c r="AB40" s="65"/>
       <c r="AC40" s="66"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="11"/>
@@ -9176,7 +9257,7 @@
       <c r="AB41" s="65"/>
       <c r="AC41" s="66"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="11"/>
@@ -9207,7 +9288,7 @@
       <c r="AB42" s="65"/>
       <c r="AC42" s="66"/>
     </row>
-    <row r="43" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="92"/>
@@ -9238,77 +9319,77 @@
       <c r="AB43" s="67"/>
       <c r="AC43" s="68"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L44" s="35"/>
       <c r="N44" s="35"/>
       <c r="O44" s="35"/>
       <c r="P44" s="35"/>
       <c r="Q44" s="35"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L45" s="35"/>
       <c r="N45" s="35"/>
       <c r="O45" s="35"/>
       <c r="P45" s="35"/>
       <c r="Q45" s="35"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L46" s="35"/>
       <c r="N46" s="35"/>
       <c r="O46" s="35"/>
       <c r="P46" s="35"/>
       <c r="Q46" s="35"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L47" s="35"/>
       <c r="N47" s="35"/>
       <c r="O47" s="35"/>
       <c r="P47" s="35"/>
       <c r="Q47" s="35"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L48" s="35"/>
       <c r="N48" s="35"/>
       <c r="O48" s="35"/>
       <c r="P48" s="35"/>
       <c r="Q48" s="35"/>
     </row>
-    <row r="49" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L49" s="35"/>
       <c r="N49" s="35"/>
       <c r="O49" s="35"/>
       <c r="P49" s="35"/>
       <c r="Q49" s="35"/>
     </row>
-    <row r="50" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L50" s="35"/>
       <c r="N50" s="35"/>
       <c r="O50" s="35"/>
       <c r="P50" s="35"/>
       <c r="Q50" s="35"/>
     </row>
-    <row r="51" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L51" s="35"/>
       <c r="N51" s="35"/>
       <c r="O51" s="35"/>
       <c r="P51" s="35"/>
       <c r="Q51" s="35"/>
     </row>
-    <row r="52" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L52" s="35"/>
       <c r="N52" s="35"/>
       <c r="O52" s="35"/>
       <c r="P52" s="35"/>
       <c r="Q52" s="35"/>
     </row>
-    <row r="53" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L53" s="35"/>
       <c r="N53" s="35"/>
       <c r="O53" s="35"/>
       <c r="P53" s="35"/>
       <c r="Q53" s="35"/>
     </row>
-    <row r="54" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L54" s="35"/>
       <c r="N54" s="35"/>
       <c r="O54" s="35"/>
@@ -9330,15 +9411,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F79E4C1-6E60-40C3-94F3-6AFDFE148649}">
-  <dimension ref="A1:Y58"/>
+  <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>487</v>
       </c>
@@ -9415,7 +9496,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>486</v>
       </c>
@@ -9492,7 +9573,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>484</v>
       </c>
@@ -9569,7 +9650,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>482</v>
       </c>
@@ -9646,7 +9727,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>480</v>
       </c>
@@ -9723,7 +9804,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>478</v>
       </c>
@@ -9800,7 +9881,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>476</v>
       </c>
@@ -9877,7 +9958,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>474</v>
       </c>
@@ -9954,7 +10035,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>472</v>
       </c>
@@ -10031,7 +10112,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>470</v>
       </c>
@@ -10108,7 +10189,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>468</v>
       </c>
@@ -10185,7 +10266,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>466</v>
       </c>
@@ -10262,7 +10343,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>464</v>
       </c>
@@ -10339,7 +10420,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>461</v>
       </c>
@@ -10416,7 +10497,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>458</v>
       </c>
@@ -10493,7 +10574,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>454</v>
       </c>
@@ -10570,7 +10651,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>454</v>
       </c>
@@ -10647,7 +10728,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>450</v>
       </c>
@@ -10724,7 +10805,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>445</v>
       </c>
@@ -10801,7 +10882,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>443</v>
       </c>
@@ -10878,7 +10959,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>438</v>
       </c>
@@ -10955,7 +11036,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>433</v>
       </c>
@@ -11032,7 +11113,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>429</v>
       </c>
@@ -11109,7 +11190,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>427</v>
       </c>
@@ -11186,7 +11267,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>421</v>
       </c>
@@ -11263,7 +11344,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>420</v>
       </c>
@@ -11340,7 +11421,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>419</v>
       </c>
@@ -11417,7 +11498,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>418</v>
       </c>
@@ -11494,7 +11575,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>416</v>
       </c>
@@ -11571,7 +11652,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>415</v>
       </c>
@@ -11648,7 +11729,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>414</v>
       </c>
@@ -11725,7 +11806,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>413</v>
       </c>
@@ -11802,7 +11883,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>411</v>
       </c>
@@ -11879,7 +11960,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>409</v>
       </c>
@@ -11956,7 +12037,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>407</v>
       </c>
@@ -12033,7 +12114,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>406</v>
       </c>
@@ -12110,7 +12191,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>401</v>
       </c>
@@ -12187,7 +12268,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>400</v>
       </c>
@@ -12264,7 +12345,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>399</v>
       </c>
@@ -12341,7 +12422,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>397</v>
       </c>
@@ -12418,7 +12499,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>394</v>
       </c>
@@ -12495,7 +12576,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>393</v>
       </c>
@@ -12572,7 +12653,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>391</v>
       </c>
@@ -12649,7 +12730,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>389</v>
       </c>
@@ -12726,7 +12807,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>383</v>
       </c>
@@ -12803,7 +12884,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>381</v>
       </c>
@@ -12880,7 +12961,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>374</v>
       </c>
@@ -12957,7 +13038,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>372</v>
       </c>
@@ -13034,7 +13115,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>370</v>
       </c>
@@ -13111,7 +13192,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>367</v>
       </c>
@@ -13188,7 +13269,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>362</v>
       </c>
@@ -13265,7 +13346,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>360</v>
       </c>
@@ -13336,7 +13417,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>540</v>
       </c>
@@ -13407,7 +13488,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>538</v>
       </c>
@@ -13478,7 +13559,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>536</v>
       </c>
@@ -13549,7 +13630,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>533</v>
       </c>
@@ -13620,7 +13701,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>528</v>
       </c>
@@ -13691,7 +13772,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>522</v>
       </c>
@@ -13760,6 +13841,670 @@
       </c>
       <c r="W58" t="s">
         <v>512</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>567</v>
+      </c>
+      <c r="B59" t="s">
+        <v>566</v>
+      </c>
+      <c r="C59" t="s">
+        <v>565</v>
+      </c>
+      <c r="D59" t="s">
+        <v>353</v>
+      </c>
+      <c r="E59" t="s">
+        <v>353</v>
+      </c>
+      <c r="F59" t="s">
+        <v>564</v>
+      </c>
+      <c r="G59" s="138">
+        <v>44741</v>
+      </c>
+      <c r="H59" t="s">
+        <v>140</v>
+      </c>
+      <c r="I59" t="s">
+        <v>187</v>
+      </c>
+      <c r="J59" t="s">
+        <v>353</v>
+      </c>
+      <c r="K59" t="s">
+        <v>353</v>
+      </c>
+      <c r="L59" t="s">
+        <v>140</v>
+      </c>
+      <c r="M59" t="s">
+        <v>187</v>
+      </c>
+      <c r="N59" t="s">
+        <v>120</v>
+      </c>
+      <c r="O59" t="s">
+        <v>516</v>
+      </c>
+      <c r="P59" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>551</v>
+      </c>
+      <c r="R59" t="s">
+        <v>494</v>
+      </c>
+      <c r="S59">
+        <v>20</v>
+      </c>
+      <c r="T59">
+        <v>40000</v>
+      </c>
+      <c r="U59">
+        <v>50000</v>
+      </c>
+      <c r="V59" t="s">
+        <v>563</v>
+      </c>
+      <c r="W59">
+        <v>1</v>
+      </c>
+      <c r="X59" t="s">
+        <v>562</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>353</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>561</v>
+      </c>
+      <c r="B60" t="s">
+        <v>532</v>
+      </c>
+      <c r="C60" t="s">
+        <v>519</v>
+      </c>
+      <c r="D60" t="s">
+        <v>553</v>
+      </c>
+      <c r="E60" t="s">
+        <v>353</v>
+      </c>
+      <c r="F60" t="s">
+        <v>560</v>
+      </c>
+      <c r="G60" s="138">
+        <v>44741</v>
+      </c>
+      <c r="H60" t="s">
+        <v>140</v>
+      </c>
+      <c r="I60" t="s">
+        <v>187</v>
+      </c>
+      <c r="J60" t="s">
+        <v>353</v>
+      </c>
+      <c r="K60" t="s">
+        <v>353</v>
+      </c>
+      <c r="L60" t="s">
+        <v>140</v>
+      </c>
+      <c r="M60" t="s">
+        <v>187</v>
+      </c>
+      <c r="N60" t="s">
+        <v>119</v>
+      </c>
+      <c r="O60" t="s">
+        <v>530</v>
+      </c>
+      <c r="P60" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>555</v>
+      </c>
+      <c r="R60" t="s">
+        <v>494</v>
+      </c>
+      <c r="S60">
+        <v>20</v>
+      </c>
+      <c r="T60">
+        <v>40000</v>
+      </c>
+      <c r="U60">
+        <v>50000</v>
+      </c>
+      <c r="V60" t="s">
+        <v>353</v>
+      </c>
+      <c r="W60" t="s">
+        <v>353</v>
+      </c>
+      <c r="X60" t="s">
+        <v>513</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>515</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>559</v>
+      </c>
+      <c r="B61" t="s">
+        <v>532</v>
+      </c>
+      <c r="C61" t="s">
+        <v>519</v>
+      </c>
+      <c r="D61" t="s">
+        <v>553</v>
+      </c>
+      <c r="E61" t="s">
+        <v>353</v>
+      </c>
+      <c r="F61" t="s">
+        <v>558</v>
+      </c>
+      <c r="G61" s="138">
+        <v>44741</v>
+      </c>
+      <c r="H61" t="s">
+        <v>140</v>
+      </c>
+      <c r="I61" t="s">
+        <v>187</v>
+      </c>
+      <c r="J61" t="s">
+        <v>353</v>
+      </c>
+      <c r="K61" t="s">
+        <v>353</v>
+      </c>
+      <c r="L61" t="s">
+        <v>140</v>
+      </c>
+      <c r="M61" t="s">
+        <v>187</v>
+      </c>
+      <c r="N61" t="s">
+        <v>119</v>
+      </c>
+      <c r="O61" t="s">
+        <v>530</v>
+      </c>
+      <c r="P61" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>551</v>
+      </c>
+      <c r="R61" t="s">
+        <v>494</v>
+      </c>
+      <c r="S61">
+        <v>20</v>
+      </c>
+      <c r="T61">
+        <v>40000</v>
+      </c>
+      <c r="U61">
+        <v>50000</v>
+      </c>
+      <c r="V61" t="s">
+        <v>353</v>
+      </c>
+      <c r="W61" t="s">
+        <v>353</v>
+      </c>
+      <c r="X61" t="s">
+        <v>513</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>515</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>557</v>
+      </c>
+      <c r="B62" t="s">
+        <v>532</v>
+      </c>
+      <c r="C62" t="s">
+        <v>519</v>
+      </c>
+      <c r="D62" t="s">
+        <v>553</v>
+      </c>
+      <c r="E62" t="s">
+        <v>353</v>
+      </c>
+      <c r="F62" t="s">
+        <v>556</v>
+      </c>
+      <c r="G62" s="138">
+        <v>44741</v>
+      </c>
+      <c r="H62" t="s">
+        <v>140</v>
+      </c>
+      <c r="I62" t="s">
+        <v>187</v>
+      </c>
+      <c r="J62" t="s">
+        <v>353</v>
+      </c>
+      <c r="K62" t="s">
+        <v>353</v>
+      </c>
+      <c r="L62" t="s">
+        <v>140</v>
+      </c>
+      <c r="M62" t="s">
+        <v>187</v>
+      </c>
+      <c r="N62" t="s">
+        <v>120</v>
+      </c>
+      <c r="O62" t="s">
+        <v>516</v>
+      </c>
+      <c r="P62" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>555</v>
+      </c>
+      <c r="R62" t="s">
+        <v>494</v>
+      </c>
+      <c r="S62">
+        <v>20</v>
+      </c>
+      <c r="T62">
+        <v>40000</v>
+      </c>
+      <c r="U62">
+        <v>50000</v>
+      </c>
+      <c r="V62" t="s">
+        <v>353</v>
+      </c>
+      <c r="W62" t="s">
+        <v>353</v>
+      </c>
+      <c r="X62" t="s">
+        <v>513</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>515</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>554</v>
+      </c>
+      <c r="B63" t="s">
+        <v>532</v>
+      </c>
+      <c r="C63" t="s">
+        <v>519</v>
+      </c>
+      <c r="D63" t="s">
+        <v>553</v>
+      </c>
+      <c r="E63" t="s">
+        <v>353</v>
+      </c>
+      <c r="F63" t="s">
+        <v>552</v>
+      </c>
+      <c r="G63" s="138">
+        <v>44741</v>
+      </c>
+      <c r="H63" t="s">
+        <v>140</v>
+      </c>
+      <c r="I63" t="s">
+        <v>187</v>
+      </c>
+      <c r="J63" t="s">
+        <v>353</v>
+      </c>
+      <c r="K63" t="s">
+        <v>353</v>
+      </c>
+      <c r="L63" t="s">
+        <v>140</v>
+      </c>
+      <c r="M63" t="s">
+        <v>187</v>
+      </c>
+      <c r="N63" t="s">
+        <v>120</v>
+      </c>
+      <c r="O63" t="s">
+        <v>516</v>
+      </c>
+      <c r="P63" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>551</v>
+      </c>
+      <c r="R63" t="s">
+        <v>494</v>
+      </c>
+      <c r="S63">
+        <v>20</v>
+      </c>
+      <c r="T63">
+        <v>40000</v>
+      </c>
+      <c r="U63">
+        <v>50000</v>
+      </c>
+      <c r="V63" t="s">
+        <v>353</v>
+      </c>
+      <c r="W63" t="s">
+        <v>353</v>
+      </c>
+      <c r="X63" t="s">
+        <v>513</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>515</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>550</v>
+      </c>
+      <c r="B64" t="s">
+        <v>545</v>
+      </c>
+      <c r="C64" t="s">
+        <v>544</v>
+      </c>
+      <c r="D64" t="s">
+        <v>543</v>
+      </c>
+      <c r="E64" t="s">
+        <v>542</v>
+      </c>
+      <c r="F64" t="s">
+        <v>549</v>
+      </c>
+      <c r="G64" s="138">
+        <v>44742</v>
+      </c>
+      <c r="H64" t="s">
+        <v>187</v>
+      </c>
+      <c r="I64" t="s">
+        <v>187</v>
+      </c>
+      <c r="J64" t="s">
+        <v>353</v>
+      </c>
+      <c r="K64" t="s">
+        <v>353</v>
+      </c>
+      <c r="L64" t="s">
+        <v>140</v>
+      </c>
+      <c r="M64" t="s">
+        <v>187</v>
+      </c>
+      <c r="N64" t="s">
+        <v>120</v>
+      </c>
+      <c r="O64" t="s">
+        <v>516</v>
+      </c>
+      <c r="P64" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>353</v>
+      </c>
+      <c r="R64" t="s">
+        <v>353</v>
+      </c>
+      <c r="S64">
+        <v>20</v>
+      </c>
+      <c r="T64">
+        <v>40000</v>
+      </c>
+      <c r="U64">
+        <v>50000</v>
+      </c>
+      <c r="V64" t="s">
+        <v>353</v>
+      </c>
+      <c r="W64" t="s">
+        <v>353</v>
+      </c>
+      <c r="X64" t="s">
+        <v>513</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>515</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>548</v>
+      </c>
+      <c r="B65" t="s">
+        <v>545</v>
+      </c>
+      <c r="C65" t="s">
+        <v>544</v>
+      </c>
+      <c r="D65" t="s">
+        <v>543</v>
+      </c>
+      <c r="E65" t="s">
+        <v>542</v>
+      </c>
+      <c r="F65" t="s">
+        <v>547</v>
+      </c>
+      <c r="G65" s="138">
+        <v>44742</v>
+      </c>
+      <c r="H65" t="s">
+        <v>140</v>
+      </c>
+      <c r="I65" t="s">
+        <v>187</v>
+      </c>
+      <c r="J65" t="s">
+        <v>353</v>
+      </c>
+      <c r="K65" t="s">
+        <v>353</v>
+      </c>
+      <c r="L65" t="s">
+        <v>140</v>
+      </c>
+      <c r="M65" t="s">
+        <v>187</v>
+      </c>
+      <c r="N65" t="s">
+        <v>120</v>
+      </c>
+      <c r="O65" t="s">
+        <v>516</v>
+      </c>
+      <c r="P65" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>353</v>
+      </c>
+      <c r="R65" t="s">
+        <v>353</v>
+      </c>
+      <c r="S65">
+        <v>20</v>
+      </c>
+      <c r="T65">
+        <v>40000</v>
+      </c>
+      <c r="U65">
+        <v>50000</v>
+      </c>
+      <c r="V65" t="s">
+        <v>353</v>
+      </c>
+      <c r="W65" t="s">
+        <v>353</v>
+      </c>
+      <c r="X65" t="s">
+        <v>513</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>515</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>546</v>
+      </c>
+      <c r="B66" t="s">
+        <v>545</v>
+      </c>
+      <c r="C66" t="s">
+        <v>544</v>
+      </c>
+      <c r="D66" t="s">
+        <v>543</v>
+      </c>
+      <c r="E66" t="s">
+        <v>542</v>
+      </c>
+      <c r="F66" t="s">
+        <v>541</v>
+      </c>
+      <c r="G66" s="138">
+        <v>44742</v>
+      </c>
+      <c r="H66" t="s">
+        <v>187</v>
+      </c>
+      <c r="I66" t="s">
+        <v>187</v>
+      </c>
+      <c r="J66" t="s">
+        <v>353</v>
+      </c>
+      <c r="K66" t="s">
+        <v>353</v>
+      </c>
+      <c r="L66" t="s">
+        <v>187</v>
+      </c>
+      <c r="M66" t="s">
+        <v>187</v>
+      </c>
+      <c r="N66" t="s">
+        <v>120</v>
+      </c>
+      <c r="O66" t="s">
+        <v>516</v>
+      </c>
+      <c r="P66" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>353</v>
+      </c>
+      <c r="R66" t="s">
+        <v>353</v>
+      </c>
+      <c r="S66">
+        <v>20</v>
+      </c>
+      <c r="T66">
+        <v>40000</v>
+      </c>
+      <c r="U66">
+        <v>50000</v>
+      </c>
+      <c r="V66" t="s">
+        <v>353</v>
+      </c>
+      <c r="W66" t="s">
+        <v>353</v>
+      </c>
+      <c r="X66" t="s">
+        <v>513</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>515</v>
+      </c>
+      <c r="AA66" t="s">
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -13775,15 +14520,15 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="96.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="96.140625" customWidth="1"/>
     <col min="4" max="4" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -13800,7 +14545,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="90">
         <v>44578</v>
       </c>
@@ -13814,7 +14559,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>44582</v>
       </c>
@@ -13831,241 +14576,241 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="105"/>
       <c r="C4" s="113"/>
       <c r="D4" s="36"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="105"/>
       <c r="C5" s="113"/>
       <c r="D5" s="37"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="105"/>
       <c r="C6" s="113"/>
       <c r="D6" s="37"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="105"/>
       <c r="C7" s="113"/>
       <c r="D7" s="37"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="105"/>
       <c r="C8" s="113"/>
       <c r="D8" s="37"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="105"/>
       <c r="C9" s="113"/>
       <c r="D9" s="37"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="105"/>
       <c r="C10" s="113"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="105"/>
       <c r="C11" s="113"/>
       <c r="D11" s="37"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="105"/>
       <c r="C12" s="113"/>
       <c r="D12" s="38"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="105"/>
       <c r="C13" s="113"/>
       <c r="D13" s="38"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="105"/>
       <c r="C14" s="113"/>
       <c r="D14" s="38"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="105"/>
       <c r="C15" s="113"/>
       <c r="D15" s="38"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="105"/>
       <c r="C16" s="113"/>
       <c r="D16" s="38"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="105"/>
       <c r="C17" s="113"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="105"/>
       <c r="C18" s="113"/>
       <c r="D18" s="38"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="105"/>
       <c r="C19" s="113"/>
       <c r="D19" s="38"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="105"/>
       <c r="C20" s="113"/>
       <c r="D20" s="38"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="105"/>
       <c r="C21" s="113"/>
       <c r="D21" s="38"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="105"/>
       <c r="C22" s="113"/>
       <c r="D22" s="38"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="105"/>
       <c r="C23" s="113"/>
       <c r="D23" s="38"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="105"/>
       <c r="C24" s="113"/>
       <c r="D24" s="38"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="105"/>
       <c r="C25" s="113"/>
       <c r="D25" s="38"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="105"/>
       <c r="C26" s="113"/>
       <c r="D26" s="38"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="105"/>
       <c r="C27" s="113"/>
       <c r="D27" s="38"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="105"/>
       <c r="C28" s="113"/>
       <c r="D28" s="38"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="105"/>
       <c r="C29" s="113"/>
       <c r="D29" s="38"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="105"/>
       <c r="C30" s="113"/>
       <c r="D30" s="38"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="105"/>
       <c r="C31" s="113"/>
       <c r="D31" s="38"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="105"/>
       <c r="C32" s="113"/>
       <c r="D32" s="38"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="105"/>
       <c r="C33" s="113"/>
       <c r="D33" s="38"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="105"/>
       <c r="C34" s="113"/>
       <c r="D34" s="38"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="105"/>
       <c r="C35" s="113"/>
       <c r="D35" s="38"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="105"/>
       <c r="C36" s="113"/>
       <c r="D36" s="38"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="105"/>
       <c r="C37" s="113"/>
       <c r="D37" s="38"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="105"/>
       <c r="C38" s="113"/>
       <c r="D38" s="38"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="105"/>
       <c r="C39" s="113"/>
       <c r="D39" s="38"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="105"/>
       <c r="C40" s="113"/>
       <c r="D40" s="38"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="105"/>
       <c r="C41" s="113"/>
       <c r="D41" s="38"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="105"/>
       <c r="C42" s="113"/>
       <c r="D42" s="38"/>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="92"/>
       <c r="B43" s="106"/>
       <c r="C43" s="114"/>
@@ -14087,20 +14832,20 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="118.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.6640625" customWidth="1"/>
-    <col min="8" max="8" width="39.6640625" customWidth="1"/>
-    <col min="9" max="9" width="49.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="118.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.7109375" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
+    <col min="9" max="9" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -14129,7 +14874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="C2" s="17" t="s">
         <v>3</v>
       </c>
@@ -14150,7 +14895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="C3" s="18" t="s">
         <v>4</v>
       </c>
@@ -14171,7 +14916,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="C4" s="18" t="s">
         <v>8</v>
       </c>
@@ -14190,7 +14935,7 @@
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>38</v>
       </c>
@@ -14217,7 +14962,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>38</v>
       </c>
@@ -14242,7 +14987,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>38</v>
       </c>
@@ -14267,7 +15012,7 @@
       </c>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>38</v>
       </c>
@@ -14296,7 +15041,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>40</v>
       </c>
@@ -14323,7 +15068,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>40</v>
       </c>
@@ -14346,7 +15091,7 @@
       <c r="H10" s="13"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>40</v>
       </c>
@@ -14369,7 +15114,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>38</v>
       </c>
@@ -14394,7 +15139,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="26"/>
       <c r="C13" s="22"/>
@@ -14405,7 +15150,7 @@
       <c r="H13" s="13"/>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>40</v>
       </c>
@@ -14430,7 +15175,7 @@
       <c r="H14" s="13"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>40</v>
       </c>
@@ -14457,7 +15202,7 @@
       </c>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>40</v>
       </c>
@@ -14484,7 +15229,7 @@
       </c>
       <c r="I16" s="14"/>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>40</v>
       </c>
@@ -14509,7 +15254,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="14"/>
     </row>
-    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>40</v>
       </c>
@@ -14536,7 +15281,7 @@
       </c>
       <c r="I18" s="34"/>
     </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>40</v>
       </c>
@@ -14563,7 +15308,7 @@
       </c>
       <c r="I19" s="34"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
         <v>40</v>
       </c>
@@ -14586,7 +15331,7 @@
       <c r="H20" s="33"/>
       <c r="I20" s="34"/>
     </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>40</v>
       </c>
@@ -14611,7 +15356,7 @@
       </c>
       <c r="I21" s="34"/>
     </row>
-    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>40</v>
       </c>
@@ -14634,7 +15379,7 @@
       <c r="H22" s="33"/>
       <c r="I22" s="34"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="29"/>
       <c r="C23" s="30"/>
@@ -14645,7 +15390,7 @@
       <c r="H23" s="33"/>
       <c r="I23" s="34"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="29"/>
       <c r="C24" s="30"/>
@@ -14656,7 +15401,7 @@
       <c r="H24" s="33"/>
       <c r="I24" s="34"/>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23"/>
       <c r="B25" s="27"/>
       <c r="C25" s="24"/>

</xml_diff>